<commit_message>
Update for graduated students data entry message
</commit_message>
<xml_diff>
--- a/student/lr.xlsx
+++ b/student/lr.xlsx
@@ -47,16 +47,16 @@
     <t>recruited</t>
   </si>
   <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>wt</t>
-  </si>
-  <si>
-    <t>Rolex</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>43</t>
+  </si>
+  <si>
+    <t>ios</t>
+  </si>
+  <si>
+    <t>Meditab Software (India) Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1122,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>

</xml_diff>